<commit_message>
change SimpleBatch default params, use one Model for examples and tests
</commit_message>
<xml_diff>
--- a/examples/SimpleBatch_Data.xlsx
+++ b/examples/SimpleBatch_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Latour\projects\estim8-s-test\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\estim8\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9BB40C-7B3E-4146-AC0A-BB960DC46257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11736"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,19 +20,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>S</t>
   </si>
   <si>
     <t>X</t>
   </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>g/L</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +54,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -53,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -76,16 +94,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -387,860 +441,875 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>0.1762</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>0.1</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>0.31831304732654309</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>0.2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.28526978766100441</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>0.3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>0.21859999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>0.4</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>0.24820963096856391</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>0.5</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>0.2684772560295704</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>0.6</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>0.3125</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>0.7</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>0.15068659507575399</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>0.8</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>0.22686999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>0.9</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>0.25814985558289438</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>0.27512580042250939</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>9.6322839099570068</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>0.36317137720520942</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>1.2</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>0.1097352844920762</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>1.3</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>8.2826792254263731E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>1.4</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>0.22987571014682501</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>1.5</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>7.1282189228621812E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>1.6</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>2.8213473465458359E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>1.7</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>0.32910068599417952</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>1.8</v>
       </c>
-      <c r="B20">
+      <c r="B21">
         <v>0.63538277979968727</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>1.9</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>0.20003427381865521</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>2</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>0.26010809085525571</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>9.706188199915502</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>2.1</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>0.12956208781409451</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>0.51818896025999361</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>0.38128147533193751</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
         <v>2.4</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>0.13491183650905739</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>2.5</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>0.3260182062275756</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>2.6</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>0.1063208458224303</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>2.7</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>0.20703591966964591</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>2.8</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>0.51466333504956085</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>2.9</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>0.43280300190202581</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>3</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>0.4448056804680931</v>
       </c>
-      <c r="C32">
+      <c r="C33">
         <v>8.9580734582815804</v>
       </c>
-      <c r="D32" s="2"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
+      <c r="D33" s="2"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>3.1</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>0.56591547090450989</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>3.2</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>0.77503894909891913</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>3.3</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>0.69783915483658121</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
         <v>3.4</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>0.27428427128878058</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>3.5</v>
       </c>
-      <c r="B37">
+      <c r="B38">
         <v>0.58985963903074379</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
         <v>3.6</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>0.62088445276081905</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
         <v>3.7</v>
       </c>
-      <c r="B39">
+      <c r="B40">
         <v>0.45950255171535698</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
         <v>3.8</v>
       </c>
-      <c r="B40">
+      <c r="B41">
         <v>0.69053527514848378</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
         <v>3.9</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>0.64893007184670859</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>4</v>
       </c>
-      <c r="B42">
+      <c r="B43">
         <v>0.61079171935120213</v>
       </c>
-      <c r="C42">
+      <c r="C43">
         <v>8.7484641460613979</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B43">
+      <c r="B44">
         <v>1.1227371555200529</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
         <v>4.1999999999999993</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>0.7289862201113122</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
         <v>4.3</v>
       </c>
-      <c r="B45">
+      <c r="B46">
         <v>0.90832376856629682</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>4.3999999999999986</v>
       </c>
-      <c r="B46">
+      <c r="B47">
         <v>1.028492178117786</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>4.4999999999999991</v>
       </c>
-      <c r="B47">
+      <c r="B48">
         <v>0.837021541987641</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="B48">
+      <c r="B49">
         <v>1.1506039733610669</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
         <v>4.6999999999999993</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>0.71321957478343267</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
         <v>4.8</v>
       </c>
-      <c r="B50">
+      <c r="B51">
         <v>0.88776325807636391</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
         <v>4.8999999999999986</v>
       </c>
-      <c r="B51">
+      <c r="B52">
         <v>0.8614157217228019</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
         <v>5</v>
       </c>
-      <c r="B52">
+      <c r="B53">
         <v>1.394123343175443</v>
       </c>
-      <c r="C52">
+      <c r="C53">
         <v>7.7941762584494061</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="B53">
+      <c r="B54">
         <v>1.815350983784604</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
         <v>5.1999999999999993</v>
       </c>
-      <c r="B54">
+      <c r="B55">
         <v>1.1412099541797169</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
         <v>5.3</v>
       </c>
-      <c r="B55">
+      <c r="B56">
         <v>1.5518658567065089</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
         <v>5.3999999999999986</v>
       </c>
-      <c r="B56">
+      <c r="B57">
         <v>1.5252218151894781</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
         <v>5.5</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>1.5667262289766131</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
         <v>5.6</v>
       </c>
-      <c r="B58">
+      <c r="B59">
         <v>1.433478500992909</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
         <v>5.6999999999999993</v>
       </c>
-      <c r="B59">
+      <c r="B60">
         <v>1.3034826971704689</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
         <v>5.8</v>
       </c>
-      <c r="B60">
+      <c r="B61">
         <v>1.892002233642073</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
         <v>5.8999999999999986</v>
       </c>
-      <c r="B61">
+      <c r="B62">
         <v>1.9717480580803559</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
         <v>6</v>
       </c>
-      <c r="B62">
+      <c r="B63">
         <v>1.952663081038593</v>
       </c>
-      <c r="C62">
+      <c r="C63">
         <v>5.9093505234403834</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
         <v>6.1</v>
       </c>
-      <c r="B63">
+      <c r="B64">
         <v>2.2945353854829058</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
         <v>6.1999999999999993</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>2.4172193192092699</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
         <v>6.3</v>
       </c>
-      <c r="B65">
+      <c r="B66">
         <v>2.512557882346496</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
         <v>6.3999999999999986</v>
       </c>
-      <c r="B66">
+      <c r="B67">
         <v>2.3058540948594382</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
         <v>6.5</v>
       </c>
-      <c r="B67">
+      <c r="B68">
         <v>2.1608194324367531</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
         <v>6.6</v>
       </c>
-      <c r="B68">
+      <c r="B69">
         <v>2.1624444751651</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
         <v>6.6999999999999993</v>
       </c>
-      <c r="B69">
+      <c r="B70">
         <v>3.091952270296161</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
         <v>6.8</v>
       </c>
-      <c r="B70">
+      <c r="B71">
         <v>3.1770047096267149</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
         <v>6.9</v>
       </c>
-      <c r="B71">
+      <c r="B72">
         <v>3.0374859505944718</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
         <v>7</v>
       </c>
-      <c r="B72">
+      <c r="B73">
         <v>3.2070090781984071</v>
       </c>
-      <c r="C72">
+      <c r="C73">
         <v>3.4435401343063212</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>7.1</v>
       </c>
-      <c r="B73">
+      <c r="B74">
         <v>3.1564923006295511</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
         <v>7.1999999999999993</v>
       </c>
-      <c r="B74">
+      <c r="B75">
         <v>3.6434062539389669</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
         <v>7.3</v>
       </c>
-      <c r="B75">
+      <c r="B76">
         <v>3.6705009624233931</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
         <v>7.4</v>
       </c>
-      <c r="B76">
+      <c r="B77">
         <v>4.1095480770708521</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
         <v>7.5</v>
       </c>
-      <c r="B77">
+      <c r="B78">
         <v>4.395046095974422</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
         <v>7.6</v>
       </c>
-      <c r="B78">
+      <c r="B79">
         <v>4.6171650196511624</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
         <v>7.6999999999999993</v>
       </c>
-      <c r="B79">
+      <c r="B80">
         <v>4.5606698398924372</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
         <v>7.8</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>4.8039335991846643</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
         <v>7.9</v>
       </c>
-      <c r="B81">
+      <c r="B82">
         <v>5.0901243182373168</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>8</v>
       </c>
-      <c r="B82">
+      <c r="B83">
         <v>5.105010141930137</v>
       </c>
-      <c r="C82">
+      <c r="C83">
         <v>1.0405288216328331E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="1">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>8.1</v>
       </c>
-      <c r="B83">
+      <c r="B84">
         <v>5.22963849501848</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="B84">
+      <c r="B85">
         <v>5.0694219071840951</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="1">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
         <v>8.2999999999999989</v>
       </c>
-      <c r="B85">
+      <c r="B86">
         <v>5.020364003863758</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="1">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
         <v>8.4</v>
       </c>
-      <c r="B86">
+      <c r="B87">
         <v>5.2640909651155336</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
         <v>8.5</v>
       </c>
-      <c r="B87">
+      <c r="B88">
         <v>5.1054344803378511</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>8.6</v>
       </c>
-      <c r="B88">
+      <c r="B89">
         <v>5.3230233413682022</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
         <v>8.6999999999999993</v>
       </c>
-      <c r="B89">
+      <c r="B90">
         <v>4.8652488655957393</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
         <v>8.7999999999999989</v>
       </c>
-      <c r="B90">
+      <c r="B91">
         <v>5.66191724665679</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
         <v>8.9</v>
       </c>
-      <c r="B91">
+      <c r="B92">
         <v>5.0055713722930486</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>9</v>
       </c>
-      <c r="B92">
+      <c r="B93">
         <v>5.1485353479574156</v>
       </c>
-      <c r="C92">
+      <c r="C93">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="1">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
         <v>9.1</v>
       </c>
-      <c r="B93">
+      <c r="B94">
         <v>4.90277401961443</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
         <v>9.1999999999999993</v>
       </c>
-      <c r="B94">
+      <c r="B95">
         <v>5.0783437507024498</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="1">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
         <v>9.2999999999999989</v>
       </c>
-      <c r="B95">
+      <c r="B96">
         <v>5.0160437499010584</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="1">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
         <v>9.4</v>
       </c>
-      <c r="B96">
+      <c r="B97">
         <v>5.1479885652684736</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="1">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
         <v>9.5</v>
       </c>
-      <c r="B97">
+      <c r="B98">
         <v>5.0799087323183798</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="1">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
         <v>9.6</v>
       </c>
-      <c r="B98">
+      <c r="B99">
         <v>4.8859555198584266</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
         <v>9.6999999999999993</v>
       </c>
-      <c r="B99">
+      <c r="B100">
         <v>4.8073508908358571</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="1">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
         <v>9.8000000000000007</v>
       </c>
-      <c r="B100">
+      <c r="B101">
         <v>5.1678742102734798</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
         <v>9.9</v>
       </c>
-      <c r="B101">
+      <c r="B102">
         <v>5.220779428233147</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="1">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
         <v>10</v>
       </c>
-      <c r="B102">
+      <c r="B103">
         <v>5.0659592497420602</v>
       </c>
-      <c r="C102">
+      <c r="C103">
         <v>0</v>
       </c>
     </row>

</xml_diff>